<commit_message>
"Try to store data in DB directly(Remove excel Files)"
</commit_message>
<xml_diff>
--- a/Maplink.xlsx
+++ b/Maplink.xlsx
@@ -2,14 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Demo_testing\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,61 +19,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
-    <t>https://www.google.co.in/maps/place/Kalapani+Museum/data=!4m7!3m6!1s0x3088941b4dbc1183:0x258764f30fb2b966!8m2!3d11.6147675!4d92.7039841!16s%2Fg%2F11csq9kycg!19sChIJgxG8TRuUiDARZrmyD_NkhyU?authuser=0&amp;hl=en&amp;rclk=1</t>
+    <t>https://www.google.co.in/maps/place/My+Art+Gallary/data=!4m7!3m6!1s0x390ce5e7cce45dd5:0xad1c1016086fd11b!8m2!3d28.5821195!4d77.3266991!16s%2Fg%2F11rst3b1yv!19sChIJ1V3kzOflDDkRG9FvCBYQHK0?authuser=0&amp;hl=en&amp;rclk=1</t>
   </si>
   <si>
-    <t>https://www.google.co.in/maps/place/Post+office/data=!4m7!3m6!1s0x30889351f3fffd6d:0x6d0b8c3df70bcb3b!8m2!3d11.6002564!4d92.7182978!16s%2Fg%2F11qbf0nd8v!19sChIJbf3_81GTiDARO8sL9z2MC20?authuser=0&amp;hl=en&amp;rclk=1</t>
+    <t>https://www.google.co.in/maps/place/Japingka+Aboriginal+Art/data=!4m7!3m6!1s0x2a32a170196dc9c7:0x1d72bcd4480b9178!8m2!3d-32.055214!4d115.7444264!16s%2Fg%2F1v6gbjsr!19sChIJx8ltGXChMioReJELSNS8ch0?authuser=0&amp;hl=en&amp;rclk=1</t>
   </si>
   <si>
-    <t>https://www.google.co.in/maps/place/Freggie+Mart+%E2%84%A2/data=!4m7!3m6!1s0x30889415f3a354bd:0xea4f4c14b7d81b74!8m2!3d11.6231824!4d92.7161393!16s%2Fg%2F11cjj_7lmy!19sChIJvVSj8xWUiDARdBvYtxRMT-o?authuser=0&amp;hl=en&amp;rclk=1</t>
+    <t>https://www.google.co.in/maps/place/Rebecca+Hossack+Art+Gallery/data=!4m7!3m6!1s0x48761b2c134a2431:0x5a72d39e5c1bed17!8m2!3d51.5220363!4d-0.139547!16s%2Fg%2F1td5wn6m!19sChIJMSRKEywbdkgRF-0bXJ7Tclo?authuser=0&amp;hl=en&amp;rclk=1</t>
   </si>
   <si>
-    <t>https://www.google.co.in/maps/place/Minnie+Bay+Post+Office/data=!4m7!3m6!1s0x30889448d99d7d33:0xbdffaeed63a06a4a!8m2!3d11.639662!4d92.722469!16s%2Fg%2F11gchx9j2s!19sChIJM32d2UiUiDARSmqgY-2u_70?authuser=0&amp;hl=en&amp;rclk=1</t>
-  </si>
-  <si>
-    <t>https://www.google.co.in/maps/place/Head+Post+Office+Port+Blair/data=!4m7!3m6!1s0x3088950bd1398657:0xd88520c4c969972f!8m2!3d11.6660012!4d92.7412679!16s%2Fg%2F1tdhprkj!19sChIJV4Y50QuViDARL5dpycQghdg?authuser=0&amp;hl=en&amp;rclk=1</t>
-  </si>
-  <si>
-    <t>https://www.google.co.in/maps/place/Voice+of+Christ+to+the+world/data=!4m7!3m6!1s0x3088958fe78c4491:0xad4015ab0fab7080!8m2!3d11.6165625!4d92.7083125!16s%2Fg%2F11swj3r51n!19sChIJkUSM54-ViDARgHCrD6sVQK0?authuser=0&amp;hl=en&amp;rclk=1</t>
-  </si>
-  <si>
-    <t>https://www.google.co.in/maps/place/Port+Blair+Tour+Package/data=!4m7!3m6!1s0x3088945c0e14ed53:0xbfac4daf5a9cc921!8m2!3d11.6307157!4d92.7323234!16s%2Fg%2F11bzv2ql7_!19sChIJU-0UDlyUiDARIcmcWq9NrL8?authuser=0&amp;hl=en&amp;rclk=1</t>
-  </si>
-  <si>
-    <t>https://www.google.co.in/maps/place/Havelock+Island+tours/data=!4m7!3m6!1s0x308895983eb27473:0x968fd7655d68fea0!8m2!3d11.6161416!4d92.7463594!16s%2Fg%2F11tf2l8rb1!19sChIJc3SyPpiViDARoP5oXWXXj5Y?authuser=0&amp;hl=en&amp;rclk=1</t>
-  </si>
-  <si>
-    <t>https://www.google.co.in/maps/place/Andaman+Yatra/data=!4m7!3m6!1s0x308895056d9509a7:0x7a183f67c38fe0f6!8m2!3d11.65826!4d92.745765!16s%2Fg%2F11b86jd9hg!19sChIJpwmVbQWViDAR9uCPw2c_GHo?authuser=0&amp;hl=en&amp;rclk=1</t>
-  </si>
-  <si>
-    <t>https://www.google.co.in/maps/place/VLP%26CO/data=!4m7!3m6!1s0x308895625e16fedb:0x3b7bb2497a572e1d!8m2!3d11.6609229!4d92.7316321!16s%2Fg%2F11fd4blcjv!19sChIJ2_4WXmKViDARHS5Xekmyezs?authuser=0&amp;hl=en&amp;rclk=1</t>
-  </si>
-  <si>
-    <t>https://www.google.co.in/maps/place/Muthoot+FinCorp+Gold+Loan/data=!4m7!3m6!1s0x308895f8de81b4e5:0x81c5157cf58320eb!8m2!3d11.6223241!4d92.7165149!16s%2Fg%2F11f7309hg6!19sChIJ5bSB3viViDAR6yCD9XwVxYE?authuser=0&amp;hl=en&amp;rclk=1</t>
-  </si>
-  <si>
-    <t>https://www.google.co.in/maps/place/Muthoot+FinCorp+Gold+Loan/data=!4m7!3m6!1s0x3088959dd460dac1:0xa06d3869ee4557d8!8m2!3d11.6700238!4d92.6519272!16s%2Fg%2F11f6ngcyt3!19sChIJwdpg1J2ViDAR2FdF7mk4baA?authuser=0&amp;hl=en&amp;rclk=1</t>
-  </si>
-  <si>
-    <t>https://www.google.co.in/maps/place/Shiv+Temple/data=!4m7!3m6!1s0x3088955d0c34875b:0xc1011185b1888ba5!8m2!3d11.6547601!4d92.7243377!16s%2Fg%2F11pkf6q83z!19sChIJW4c0DF2ViDARpYuIsYURAcE?authuser=0&amp;hl=en&amp;rclk=1</t>
-  </si>
-  <si>
-    <t>https://www.google.co.in/maps/place/Axis+Bank+Branch/data=!4m7!3m6!1s0x308895a6be5db5f9:0x12b803ee4eaa69eb!8m2!3d11.666814!4d92.733406!16s%2Fg%2F1twxnxd3!19sChIJ-bVdvqaViDAR62mqTu4DuBI?authuser=0&amp;hl=en&amp;rclk=1</t>
+    <t>Aboriginal art gallery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,13 +70,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -383,90 +359,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B1" sqref="B1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="228.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>